<commit_message>
User authentication and review system added
</commit_message>
<xml_diff>
--- a/media/report.xlsx
+++ b/media/report.xlsx
@@ -375,7 +375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,17 +495,17 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>06-25-2020</t>
+          <t>06-30-2020</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Mr. Braham Prakash Tripathi</t>
+          <t>Mr. B P Tripathi</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>11 ABC</t>
+          <t>III B</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -514,17 +514,17 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>Hello World</t>
+          <t>Give and Take</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr">
@@ -534,45 +534,45 @@
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>Various things</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="n"/>
+          <t>Quiz</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr"/>
       <c r="L4" s="2" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>06-25-2020</t>
+          <t>06-30-2020</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>Mr. Braham Prakash Tripathi</t>
+          <t>Mr. Ashok Uttam</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>3 ABC</t>
+          <t>V B</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Maths</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>Numbers</t>
+          <t>OOPs</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
@@ -582,156 +582,15 @@
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>Quiz
-Worksheet</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="n"/>
+          <t>Sth</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>Keep It Up</t>
+        </is>
+      </c>
       <c r="L5" s="2" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>06-25-2020</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Mr. S K Dixit</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>4 ABC</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>63</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>Verb</t>
-        </is>
-      </c>
-      <c r="I6" s="2" t="inlineStr">
-        <is>
-          <t>WhatsApp</t>
-        </is>
-      </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>Assignment</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="n"/>
-      <c r="L6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>06-25-2020</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>Mr. Braham Prakash Tripathi</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>3 A</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Maths</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="H7" s="2" t="inlineStr">
-        <is>
-          <t>long</t>
-        </is>
-      </c>
-      <c r="I7" s="2" t="inlineStr">
-        <is>
-          <t>zoom</t>
-        </is>
-      </c>
-      <c r="J7" s="2" t="inlineStr">
-        <is>
-          <t>ram ram</t>
-        </is>
-      </c>
-      <c r="K7" s="2" t="n"/>
-      <c r="L7" s="2" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>06-25-2020</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Mr. Braham Prakash Tripathi</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>10 C</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>EVS</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>120</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>70</v>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>acvfv</t>
-        </is>
-      </c>
-      <c r="I8" s="2" t="inlineStr">
-        <is>
-          <t>Zoom</t>
-        </is>
-      </c>
-      <c r="J8" s="2" t="inlineStr">
-        <is>
-          <t>quiz</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="n"/>
-      <c r="L8" s="2" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>